<commit_message>
Changes in data files
</commit_message>
<xml_diff>
--- a/material_preparation_step/passenger_manifest_table.xlsx
+++ b/material_preparation_step/passenger_manifest_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avkashchauhan99/work/avkash/udacity/nd073-c3-building-computer-vision-solutions-with-azure-project-starter/starter/sample_manifest_table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B744AE01-3583-4320-92BA-0A3CAF704C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE9ED3BE-6DCE-430A-9044-69A95EE8C655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,10 +163,10 @@
     <t>12 Sep 2022</t>
   </si>
   <si>
-    <t>Neeha Rathna</t>
-  </si>
-  <si>
-    <t>Janjanam</t>
+    <t>Neeha</t>
+  </si>
+  <si>
+    <t>Rathna Janjanam</t>
   </si>
   <si>
     <t>4D</t>
@@ -1059,7 +1059,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>

</xml_diff>